<commit_message>
Deployed ac3a9f2 to 2023.1 with MkDocs 1.4.2 and mike 1.1.2
</commit_message>
<xml_diff>
--- a/2023.1/files/deposit/template_answers.xlsx
+++ b/2023.1/files/deposit/template_answers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seb/Documents/Codes/CERG-C/docs/files/deposit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B89139-5931-D84F-8E3C-DD34E93BA023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5EF6EE3-CD74-3443-9C61-CFFD16304C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1320" windowWidth="27240" windowHeight="16000" xr2:uid="{36F5F6DA-3494-F646-B206-C41255F24CD8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20400" xr2:uid="{36F5F6DA-3494-F646-B206-C41255F24CD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1683,8 +1683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BED1A075-1C6C-FD4A-AA11-9B92B385BC4A}">
   <dimension ref="B2:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>